<commit_message>
Simplify column logic (#6)
</commit_message>
<xml_diff>
--- a/src/ExcelsiorAspose.Tests/Tests.DisableWhitespaceTrim.verified.xlsx
+++ b/src/ExcelsiorAspose.Tests/Tests.DisableWhitespaceTrim.verified.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Employee ID</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">    john@company.com    </t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>False</t>
@@ -537,17 +534,15 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>